<commit_message>
ch-ka pompy i zaworu gornego
</commit_message>
<xml_diff>
--- a/LP/Nasze/zbiorniki_poziom_wody.xlsx
+++ b/LP/Nasze/zbiorniki_poziom_wody.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia_repo\studia\LP\Nasze\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Zbiornik1</t>
   </si>
@@ -37,12 +42,33 @@
   </si>
   <si>
     <t>zawor3</t>
+  </si>
+  <si>
+    <t>52s</t>
+  </si>
+  <si>
+    <t>czas do 5 cm</t>
+  </si>
+  <si>
+    <t>wymiary zbiornika</t>
+  </si>
+  <si>
+    <t>w 30: 41.5</t>
+  </si>
+  <si>
+    <t>w 5: 15.5</t>
+  </si>
+  <si>
+    <t>głębokość: 5</t>
+  </si>
+  <si>
+    <t>objętość</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,7 +103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -85,14 +111,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -130,9 +159,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -165,9 +194,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,9 +246,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -375,16 +438,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -397,17 +465,23 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -423,11 +497,41 @@
       <c r="G2">
         <v>0.2</v>
       </c>
-      <c r="I2">
+      <c r="H2">
+        <v>8.69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f>B10/144.8</f>
+        <v>26.761049723756905</v>
+      </c>
+      <c r="L2">
+        <f>C10/119.4</f>
+        <v>29.679648241206028</v>
+      </c>
+      <c r="O2">
+        <f>303.7-52</f>
+        <v>251.7</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>31</v>
+      </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -443,8 +547,50 @@
       <c r="G3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>$B$10/O3</f>
+        <v>39.899093904448101</v>
+      </c>
+      <c r="I3">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="J3">
+        <v>0.9</v>
+      </c>
+      <c r="K3">
+        <f>B10/150.6</f>
+        <v>25.730411686586987</v>
+      </c>
+      <c r="L3">
+        <f>C10/124.43</f>
+        <v>28.479868198987379</v>
+      </c>
+      <c r="O3">
+        <f>116.2-I3</f>
+        <v>97.12</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X3">
+        <f>(41.5+10)/2*5*30</f>
+        <v>3862.5</v>
+      </c>
+      <c r="Y3">
+        <f>(15.5+10)/2*5*5</f>
+        <v>318.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15</v>
       </c>
@@ -460,8 +606,26 @@
       <c r="G4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" ref="H4:H10" si="0">$B$10/O4</f>
+        <v>59.523809523809526</v>
+      </c>
+      <c r="I4">
+        <v>13.5</v>
+      </c>
+      <c r="J4">
+        <v>0.8</v>
+      </c>
+      <c r="K4">
+        <f>B10/157</f>
+        <v>24.681528662420384</v>
+      </c>
+      <c r="O4">
+        <f>78.6-I4</f>
+        <v>65.099999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -477,8 +641,26 @@
       <c r="G5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>75.965496961380126</v>
+      </c>
+      <c r="I5">
+        <v>6.79</v>
+      </c>
+      <c r="J5">
+        <v>0.7</v>
+      </c>
+      <c r="K5">
+        <f>B10/177.6</f>
+        <v>21.818693693693696</v>
+      </c>
+      <c r="O5">
+        <f>57.8-I5</f>
+        <v>51.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
@@ -494,8 +676,26 @@
       <c r="G6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>89.99071063632141</v>
+      </c>
+      <c r="I6">
+        <v>5.77</v>
+      </c>
+      <c r="J6">
+        <v>0.6</v>
+      </c>
+      <c r="K6">
+        <f>B10/214.5</f>
+        <v>18.065268065268064</v>
+      </c>
+      <c r="O6">
+        <f>48.83-I6</f>
+        <v>43.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -511,20 +711,92 @@
       <c r="G7">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>102.45901639344262</v>
+      </c>
+      <c r="I7">
+        <v>6.39</v>
+      </c>
+      <c r="J7">
+        <v>0.5</v>
+      </c>
+      <c r="K7">
+        <f>B10/265.4</f>
+        <v>14.600602863602111</v>
+      </c>
+      <c r="O7">
+        <f>44.21-I7</f>
+        <v>37.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="G8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>115.05344418052256</v>
+      </c>
+      <c r="I8">
+        <v>5.42</v>
+      </c>
+      <c r="J8">
+        <v>0.4</v>
+      </c>
+      <c r="K8">
+        <f>B10/478.9</f>
+        <v>8.0914595949049914</v>
+      </c>
+      <c r="O8">
+        <f>39.1-I8</f>
+        <v>33.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>128.26878517047334</v>
+      </c>
+      <c r="I9">
+        <v>4.49</v>
+      </c>
+      <c r="J9">
+        <v>0.3</v>
+      </c>
+      <c r="O9">
+        <f>34.7-I9</f>
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <f>25*31*5</f>
+        <v>3875</v>
+      </c>
+      <c r="C10">
+        <f>X3-Y3</f>
+        <v>3543.75</v>
+      </c>
       <c r="G10">
         <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>139.7907647907648</v>
+      </c>
+      <c r="I10">
+        <v>5.47</v>
+      </c>
+      <c r="O10">
+        <f>33.19-I10</f>
+        <v>27.72</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -546,7 +818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>